<commit_message>
Remove unnecessary functions, extra files, etc
</commit_message>
<xml_diff>
--- a/reports/modifier_impact_TS_Speck.xlsx
+++ b/reports/modifier_impact_TS_Speck.xlsx
@@ -64,28 +64,28 @@
     <t>MCC950</t>
   </si>
   <si>
-    <t>(-0.071, 1.074)</t>
-  </si>
-  <si>
-    <t>(-0.635, 0.369)</t>
+    <t>(-0.083, 1.082)</t>
+  </si>
+  <si>
+    <t>(-0.65, 0.375)</t>
   </si>
   <si>
     <t>MSU</t>
   </si>
   <si>
-    <t>(1.452, 3.938)</t>
-  </si>
-  <si>
-    <t>(-0.654, 0.246)</t>
+    <t>(1.457, 3.912)</t>
+  </si>
+  <si>
+    <t>(-0.658, 0.239)</t>
   </si>
   <si>
     <t>Nigericin</t>
   </si>
   <si>
-    <t>(11.647, 54.499)</t>
-  </si>
-  <si>
-    <t>(1.081, 14.033)</t>
+    <t>(11.535, 54.613)</t>
+  </si>
+  <si>
+    <t>(1.086, 13.933)</t>
   </si>
 </sst>
 </file>
@@ -510,13 +510,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.108</v>
+        <v>0.121</v>
       </c>
       <c r="C5">
-        <v>0.012</v>
+        <v>0.003</v>
       </c>
       <c r="D5">
-        <v>0.003</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -594,10 +594,10 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.003</v>
+        <v>0.007</v>
       </c>
       <c r="C11">
-        <v>0.001</v>
+        <v>0.002</v>
       </c>
       <c r="D11">
         <v>0.012</v>

</xml_diff>